<commit_message>
Input Update To New Data
</commit_message>
<xml_diff>
--- a/input-data/quietness_score_maker.xlsx
+++ b/input-data/quietness_score_maker.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="38">
   <si>
     <t>highway</t>
   </si>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2882,9 +2882,18 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D130" t="e">
+      <c r="A130" t="s">
+        <v>16</v>
+      </c>
+      <c r="B130" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" t="s">
+        <v>29</v>
+      </c>
+      <c r="D130">
         <f>Generator!$D130</f>
-        <v>#N/A</v>
+        <v>75</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -4881,8 +4890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H400"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C400"/>
+    <sheetView topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="B400" sqref="B400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9266,37 +9275,37 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130">
+      <c r="A130" t="str">
         <f>quietness!A130</f>
-        <v>0</v>
-      </c>
-      <c r="B130">
+        <v>road</v>
+      </c>
+      <c r="B130" t="str">
         <f>quietness!B130</f>
-        <v>0</v>
-      </c>
-      <c r="C130">
+        <v>share_busway</v>
+      </c>
+      <c r="C130" t="str">
         <f>quietness!C130</f>
-        <v>0</v>
-      </c>
-      <c r="D130" t="e">
+        <v>no</v>
+      </c>
+      <c r="D130">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E130" t="e">
+        <v>75</v>
+      </c>
+      <c r="E130">
         <f>VLOOKUP($A130,Rules!$A$4:$B$50,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F130" t="e">
+        <v>70</v>
+      </c>
+      <c r="F130">
         <f>VLOOKUP($B130,Rules!$D$4:$E$10,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G130" t="e">
+        <v>5</v>
+      </c>
+      <c r="G130">
         <f>VLOOKUP($C130,Rules!$D$4:$E$10,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H130" t="e">
+        <v>0</v>
+      </c>
+      <c r="H130">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>75</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>